<commit_message>
add 3 big programmes
</commit_message>
<xml_diff>
--- a/3_2_multi_programmes_detect/data/detect.111432/111432实验结果.xlsx
+++ b/3_2_multi_programmes_detect/data/detect.111432/111432实验结果.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>样本</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -66,29 +67,67 @@
   <si>
     <t>malware</t>
   </si>
+  <si>
+    <t>Malware</t>
+  </si>
+  <si>
+    <t>Jevereg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Secondwrite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cholesky</t>
+  </si>
+  <si>
+    <t>lu-c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lu-nc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ocean-c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ocean-nc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>water-n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>water-s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -102,7 +141,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -110,17 +149,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -404,24 +472,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H229"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="12.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="12.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.125" style="2"/>
+    <col min="5" max="5" width="12.875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +509,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -461,7 +529,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -481,7 +549,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -501,7 +569,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -521,7 +589,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -541,7 +609,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -561,7 +629,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -581,7 +649,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -601,7 +669,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -621,7 +689,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -631,7 +699,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -641,7 +709,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -651,7 +719,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -661,7 +729,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -671,7 +739,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -681,7 +749,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -691,7 +759,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -701,7 +769,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -711,7 +779,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -721,7 +789,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -731,7 +799,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -741,7 +809,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -751,7 +819,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -761,7 +829,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -771,7 +839,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -781,7 +849,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -791,7 +859,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -801,7 +869,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -811,7 +879,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -821,7 +889,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -831,7 +899,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -841,7 +909,7 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -851,7 +919,7 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -861,7 +929,7 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -871,7 +939,7 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -881,7 +949,7 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -891,7 +959,7 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -901,7 +969,7 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -911,7 +979,7 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -921,7 +989,7 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -931,7 +999,7 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -941,7 +1009,7 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -951,7 +1019,7 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -961,7 +1029,7 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -971,7 +1039,7 @@
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -981,7 +1049,7 @@
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -991,7 +1059,7 @@
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1001,7 +1069,7 @@
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1011,7 +1079,7 @@
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1021,7 +1089,7 @@
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1031,7 +1099,7 @@
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1041,7 +1109,7 @@
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1051,7 +1119,7 @@
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1061,7 +1129,7 @@
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1071,7 +1139,7 @@
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1081,7 +1149,7 @@
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1091,7 +1159,7 @@
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1101,7 +1169,7 @@
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1111,7 +1179,7 @@
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1121,7 +1189,7 @@
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1131,7 +1199,7 @@
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1141,7 +1209,7 @@
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1151,7 +1219,7 @@
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1161,7 +1229,7 @@
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1171,7 +1239,7 @@
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1181,7 +1249,7 @@
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1191,7 +1259,7 @@
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1201,7 +1269,7 @@
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1211,7 +1279,7 @@
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1221,7 +1289,7 @@
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1231,7 +1299,7 @@
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1241,7 +1309,7 @@
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1251,7 +1319,7 @@
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1261,7 +1329,7 @@
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1271,7 +1339,7 @@
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1281,7 +1349,7 @@
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1291,7 +1359,7 @@
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1301,7 +1369,7 @@
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1311,7 +1379,7 @@
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1321,7 +1389,7 @@
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -1331,7 +1399,7 @@
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1341,7 +1409,7 @@
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -1351,7 +1419,7 @@
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -1361,7 +1429,7 @@
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -1371,7 +1439,7 @@
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -1381,7 +1449,7 @@
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -1391,7 +1459,7 @@
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -1401,7 +1469,7 @@
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -1411,7 +1479,7 @@
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -1421,7 +1489,7 @@
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -1431,7 +1499,7 @@
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -1441,7 +1509,7 @@
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -1451,7 +1519,7 @@
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -1461,7 +1529,7 @@
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -1471,7 +1539,7 @@
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -1481,7 +1549,7 @@
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -1491,7 +1559,7 @@
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -1501,7 +1569,7 @@
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -1511,7 +1579,7 @@
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -1521,7 +1589,7 @@
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -1531,7 +1599,7 @@
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -1541,7 +1609,7 @@
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -1551,7 +1619,7 @@
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -1561,7 +1629,7 @@
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -1571,7 +1639,7 @@
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -1581,7 +1649,7 @@
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -1591,7 +1659,7 @@
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -1601,7 +1669,7 @@
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -1611,7 +1679,7 @@
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -1621,7 +1689,7 @@
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -1631,7 +1699,7 @@
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -1641,7 +1709,7 @@
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -1651,7 +1719,7 @@
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -1661,7 +1729,7 @@
       <c r="G114" s="1"/>
       <c r="H114" s="1"/>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -1671,7 +1739,7 @@
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -1681,7 +1749,7 @@
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -1691,7 +1759,7 @@
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -1701,7 +1769,7 @@
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -1711,7 +1779,7 @@
       <c r="G119" s="1"/>
       <c r="H119" s="1"/>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -1721,7 +1789,7 @@
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -1731,7 +1799,7 @@
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -1741,7 +1809,7 @@
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -1751,7 +1819,7 @@
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -1761,7 +1829,7 @@
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -1771,7 +1839,7 @@
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -1781,7 +1849,7 @@
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -1791,7 +1859,7 @@
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -1801,7 +1869,7 @@
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -1811,7 +1879,7 @@
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -1821,7 +1889,7 @@
       <c r="G130" s="1"/>
       <c r="H130" s="1"/>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -1831,7 +1899,7 @@
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -1841,7 +1909,7 @@
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -1851,7 +1919,7 @@
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -1861,7 +1929,7 @@
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -1871,7 +1939,7 @@
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -1881,7 +1949,7 @@
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -1891,7 +1959,7 @@
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -1901,7 +1969,7 @@
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -1911,7 +1979,7 @@
       <c r="G139" s="1"/>
       <c r="H139" s="1"/>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -1921,7 +1989,7 @@
       <c r="G140" s="1"/>
       <c r="H140" s="1"/>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -1931,7 +1999,7 @@
       <c r="G141" s="1"/>
       <c r="H141" s="1"/>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -1941,7 +2009,7 @@
       <c r="G142" s="1"/>
       <c r="H142" s="1"/>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -1951,7 +2019,7 @@
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -1961,7 +2029,7 @@
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -1971,7 +2039,7 @@
       <c r="G145" s="1"/>
       <c r="H145" s="1"/>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -1981,7 +2049,7 @@
       <c r="G146" s="1"/>
       <c r="H146" s="1"/>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -1991,7 +2059,7 @@
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -2001,7 +2069,7 @@
       <c r="G148" s="1"/>
       <c r="H148" s="1"/>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -2011,7 +2079,7 @@
       <c r="G149" s="1"/>
       <c r="H149" s="1"/>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -2021,7 +2089,7 @@
       <c r="G150" s="1"/>
       <c r="H150" s="1"/>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -2031,7 +2099,7 @@
       <c r="G151" s="1"/>
       <c r="H151" s="1"/>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -2041,7 +2109,7 @@
       <c r="G152" s="1"/>
       <c r="H152" s="1"/>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -2051,7 +2119,7 @@
       <c r="G153" s="1"/>
       <c r="H153" s="1"/>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -2061,7 +2129,7 @@
       <c r="G154" s="1"/>
       <c r="H154" s="1"/>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -2071,7 +2139,7 @@
       <c r="G155" s="1"/>
       <c r="H155" s="1"/>
     </row>
-    <row r="156" spans="1:8">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -2081,7 +2149,7 @@
       <c r="G156" s="1"/>
       <c r="H156" s="1"/>
     </row>
-    <row r="157" spans="1:8">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -2091,7 +2159,7 @@
       <c r="G157" s="1"/>
       <c r="H157" s="1"/>
     </row>
-    <row r="158" spans="1:8">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -2101,7 +2169,7 @@
       <c r="G158" s="1"/>
       <c r="H158" s="1"/>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -2111,7 +2179,7 @@
       <c r="G159" s="1"/>
       <c r="H159" s="1"/>
     </row>
-    <row r="160" spans="1:8">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -2121,7 +2189,7 @@
       <c r="G160" s="1"/>
       <c r="H160" s="1"/>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -2131,7 +2199,7 @@
       <c r="G161" s="1"/>
       <c r="H161" s="1"/>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -2141,7 +2209,7 @@
       <c r="G162" s="1"/>
       <c r="H162" s="1"/>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -2151,7 +2219,7 @@
       <c r="G163" s="1"/>
       <c r="H163" s="1"/>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -2161,7 +2229,7 @@
       <c r="G164" s="1"/>
       <c r="H164" s="1"/>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -2171,7 +2239,7 @@
       <c r="G165" s="1"/>
       <c r="H165" s="1"/>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -2181,7 +2249,7 @@
       <c r="G166" s="1"/>
       <c r="H166" s="1"/>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -2191,7 +2259,7 @@
       <c r="G167" s="1"/>
       <c r="H167" s="1"/>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -2201,7 +2269,7 @@
       <c r="G168" s="1"/>
       <c r="H168" s="1"/>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -2211,7 +2279,7 @@
       <c r="G169" s="1"/>
       <c r="H169" s="1"/>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -2221,7 +2289,7 @@
       <c r="G170" s="1"/>
       <c r="H170" s="1"/>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -2231,7 +2299,7 @@
       <c r="G171" s="1"/>
       <c r="H171" s="1"/>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -2241,7 +2309,7 @@
       <c r="G172" s="1"/>
       <c r="H172" s="1"/>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -2251,7 +2319,7 @@
       <c r="G173" s="1"/>
       <c r="H173" s="1"/>
     </row>
-    <row r="174" spans="1:8">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -2261,7 +2329,7 @@
       <c r="G174" s="1"/>
       <c r="H174" s="1"/>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -2271,7 +2339,7 @@
       <c r="G175" s="1"/>
       <c r="H175" s="1"/>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -2281,7 +2349,7 @@
       <c r="G176" s="1"/>
       <c r="H176" s="1"/>
     </row>
-    <row r="177" spans="1:8">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -2291,7 +2359,7 @@
       <c r="G177" s="1"/>
       <c r="H177" s="1"/>
     </row>
-    <row r="178" spans="1:8">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -2301,7 +2369,7 @@
       <c r="G178" s="1"/>
       <c r="H178" s="1"/>
     </row>
-    <row r="179" spans="1:8">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -2311,7 +2379,7 @@
       <c r="G179" s="1"/>
       <c r="H179" s="1"/>
     </row>
-    <row r="180" spans="1:8">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -2321,7 +2389,7 @@
       <c r="G180" s="1"/>
       <c r="H180" s="1"/>
     </row>
-    <row r="181" spans="1:8">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -2331,7 +2399,7 @@
       <c r="G181" s="1"/>
       <c r="H181" s="1"/>
     </row>
-    <row r="182" spans="1:8">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -2341,7 +2409,7 @@
       <c r="G182" s="1"/>
       <c r="H182" s="1"/>
     </row>
-    <row r="183" spans="1:8">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -2351,7 +2419,7 @@
       <c r="G183" s="1"/>
       <c r="H183" s="1"/>
     </row>
-    <row r="184" spans="1:8">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -2361,7 +2429,7 @@
       <c r="G184" s="1"/>
       <c r="H184" s="1"/>
     </row>
-    <row r="185" spans="1:8">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -2371,7 +2439,7 @@
       <c r="G185" s="1"/>
       <c r="H185" s="1"/>
     </row>
-    <row r="186" spans="1:8">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -2381,7 +2449,7 @@
       <c r="G186" s="1"/>
       <c r="H186" s="1"/>
     </row>
-    <row r="187" spans="1:8">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -2391,7 +2459,7 @@
       <c r="G187" s="1"/>
       <c r="H187" s="1"/>
     </row>
-    <row r="188" spans="1:8">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -2401,7 +2469,7 @@
       <c r="G188" s="1"/>
       <c r="H188" s="1"/>
     </row>
-    <row r="189" spans="1:8">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -2411,7 +2479,7 @@
       <c r="G189" s="1"/>
       <c r="H189" s="1"/>
     </row>
-    <row r="190" spans="1:8">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -2421,7 +2489,7 @@
       <c r="G190" s="1"/>
       <c r="H190" s="1"/>
     </row>
-    <row r="191" spans="1:8">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -2431,7 +2499,7 @@
       <c r="G191" s="1"/>
       <c r="H191" s="1"/>
     </row>
-    <row r="192" spans="1:8">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -2441,7 +2509,7 @@
       <c r="G192" s="1"/>
       <c r="H192" s="1"/>
     </row>
-    <row r="193" spans="1:8">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -2451,7 +2519,7 @@
       <c r="G193" s="1"/>
       <c r="H193" s="1"/>
     </row>
-    <row r="194" spans="1:8">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -2461,7 +2529,7 @@
       <c r="G194" s="1"/>
       <c r="H194" s="1"/>
     </row>
-    <row r="195" spans="1:8">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -2471,7 +2539,7 @@
       <c r="G195" s="1"/>
       <c r="H195" s="1"/>
     </row>
-    <row r="196" spans="1:8">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -2481,7 +2549,7 @@
       <c r="G196" s="1"/>
       <c r="H196" s="1"/>
     </row>
-    <row r="197" spans="1:8">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -2491,7 +2559,7 @@
       <c r="G197" s="1"/>
       <c r="H197" s="1"/>
     </row>
-    <row r="198" spans="1:8">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -2501,7 +2569,7 @@
       <c r="G198" s="1"/>
       <c r="H198" s="1"/>
     </row>
-    <row r="199" spans="1:8">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -2511,7 +2579,7 @@
       <c r="G199" s="1"/>
       <c r="H199" s="1"/>
     </row>
-    <row r="200" spans="1:8">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -2521,7 +2589,7 @@
       <c r="G200" s="1"/>
       <c r="H200" s="1"/>
     </row>
-    <row r="201" spans="1:8">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -2531,7 +2599,7 @@
       <c r="G201" s="1"/>
       <c r="H201" s="1"/>
     </row>
-    <row r="202" spans="1:8">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -2541,7 +2609,7 @@
       <c r="G202" s="1"/>
       <c r="H202" s="1"/>
     </row>
-    <row r="203" spans="1:8">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -2551,7 +2619,7 @@
       <c r="G203" s="1"/>
       <c r="H203" s="1"/>
     </row>
-    <row r="204" spans="1:8">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -2561,7 +2629,7 @@
       <c r="G204" s="1"/>
       <c r="H204" s="1"/>
     </row>
-    <row r="205" spans="1:8">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
@@ -2571,7 +2639,7 @@
       <c r="G205" s="1"/>
       <c r="H205" s="1"/>
     </row>
-    <row r="206" spans="1:8">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
@@ -2581,7 +2649,7 @@
       <c r="G206" s="1"/>
       <c r="H206" s="1"/>
     </row>
-    <row r="207" spans="1:8">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
@@ -2591,7 +2659,7 @@
       <c r="G207" s="1"/>
       <c r="H207" s="1"/>
     </row>
-    <row r="208" spans="1:8">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
@@ -2601,7 +2669,7 @@
       <c r="G208" s="1"/>
       <c r="H208" s="1"/>
     </row>
-    <row r="209" spans="1:8">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
@@ -2611,7 +2679,7 @@
       <c r="G209" s="1"/>
       <c r="H209" s="1"/>
     </row>
-    <row r="210" spans="1:8">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" s="1"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
@@ -2621,7 +2689,7 @@
       <c r="G210" s="1"/>
       <c r="H210" s="1"/>
     </row>
-    <row r="211" spans="1:8">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" s="1"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
@@ -2631,7 +2699,7 @@
       <c r="G211" s="1"/>
       <c r="H211" s="1"/>
     </row>
-    <row r="212" spans="1:8">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" s="1"/>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
@@ -2641,7 +2709,7 @@
       <c r="G212" s="1"/>
       <c r="H212" s="1"/>
     </row>
-    <row r="213" spans="1:8">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" s="1"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
@@ -2651,7 +2719,7 @@
       <c r="G213" s="1"/>
       <c r="H213" s="1"/>
     </row>
-    <row r="214" spans="1:8">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" s="1"/>
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
@@ -2661,7 +2729,7 @@
       <c r="G214" s="1"/>
       <c r="H214" s="1"/>
     </row>
-    <row r="215" spans="1:8">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" s="1"/>
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
@@ -2671,7 +2739,7 @@
       <c r="G215" s="1"/>
       <c r="H215" s="1"/>
     </row>
-    <row r="216" spans="1:8">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216" s="1"/>
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
@@ -2681,7 +2749,7 @@
       <c r="G216" s="1"/>
       <c r="H216" s="1"/>
     </row>
-    <row r="217" spans="1:8">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217" s="1"/>
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
@@ -2691,7 +2759,7 @@
       <c r="G217" s="1"/>
       <c r="H217" s="1"/>
     </row>
-    <row r="218" spans="1:8">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" s="1"/>
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
@@ -2701,7 +2769,7 @@
       <c r="G218" s="1"/>
       <c r="H218" s="1"/>
     </row>
-    <row r="219" spans="1:8">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219" s="1"/>
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
@@ -2711,7 +2779,7 @@
       <c r="G219" s="1"/>
       <c r="H219" s="1"/>
     </row>
-    <row r="220" spans="1:8">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A220" s="1"/>
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
@@ -2721,7 +2789,7 @@
       <c r="G220" s="1"/>
       <c r="H220" s="1"/>
     </row>
-    <row r="221" spans="1:8">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" s="1"/>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
@@ -2731,7 +2799,7 @@
       <c r="G221" s="1"/>
       <c r="H221" s="1"/>
     </row>
-    <row r="222" spans="1:8">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" s="1"/>
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
@@ -2741,7 +2809,7 @@
       <c r="G222" s="1"/>
       <c r="H222" s="1"/>
     </row>
-    <row r="223" spans="1:8">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A223" s="1"/>
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
@@ -2751,7 +2819,7 @@
       <c r="G223" s="1"/>
       <c r="H223" s="1"/>
     </row>
-    <row r="224" spans="1:8">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A224" s="1"/>
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
@@ -2761,7 +2829,7 @@
       <c r="G224" s="1"/>
       <c r="H224" s="1"/>
     </row>
-    <row r="225" spans="1:8">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" s="1"/>
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
@@ -2771,7 +2839,7 @@
       <c r="G225" s="1"/>
       <c r="H225" s="1"/>
     </row>
-    <row r="226" spans="1:8">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226" s="1"/>
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
@@ -2781,7 +2849,7 @@
       <c r="G226" s="1"/>
       <c r="H226" s="1"/>
     </row>
-    <row r="227" spans="1:8">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A227" s="1"/>
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
@@ -2791,7 +2859,7 @@
       <c r="G227" s="1"/>
       <c r="H227" s="1"/>
     </row>
-    <row r="228" spans="1:8">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" s="1"/>
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
@@ -2801,7 +2869,7 @@
       <c r="G228" s="1"/>
       <c r="H228" s="1"/>
     </row>
-    <row r="229" spans="1:8">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A229" s="1"/>
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
@@ -2816,4 +2884,131 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>